<commit_message>
Lots of PDF Report generated Page updated. Fertilizer Recommendations dataset is now fixed. Main GUI Logos added. Datasets updated.
</commit_message>
<xml_diff>
--- a/Test Reports/2154_test.xlsx
+++ b/Test Reports/2154_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,6 +522,11 @@
           <t>Recommendations</t>
         </is>
       </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Fertilizer Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -531,71 +536,76 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10-04-2024</t>
+          <t>11-04-2024</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>566</v>
+        <v>546</v>
       </c>
       <c r="D2" t="n">
-        <v>656</v>
+        <v>545</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>asdasjdhklasd</t>
+          <t>asdjhalksdjkl</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>121as2d31asd</t>
+          <t>214asd45asd65</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>6695659658</t>
+          <t>8797865461</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="L2" t="n">
-        <v>252</v>
+        <v>154</v>
       </c>
       <c r="M2" t="n">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="N2" t="n">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="O2" t="n">
         <v>2</v>
       </c>
       <c r="P2" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="Q2" t="n">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="R2" t="n">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="S2" t="n">
-        <v>0.3521566882991638</v>
+        <v>0.568192230958883</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Grow millets (sorghum, pearl millet), pulses (pigeon pea, chickpea), and oilseeds (safflower, castor).</t>
+          <t>Grow maize, soybean, groundnut, cotton, and incorporate legumes into the cropping system.</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Apply organic amendments like Compost (2-3 tonnes/ha), Vermicompost (1-1.5 tonnes/ha), or Well-decomposed Farmyard manure (5-7.5 tonnes/ha). Use biofertilizers like Rhizobium (200-300 g/ha), Azotobacter (200-300 g/ha), and PSB (500-750 g/ha). Apply chemical fertilizers at 75% of the recommended dose based on soil test results and crop requirements.</t>
         </is>
       </c>
     </row>

</xml_diff>